<commit_message>
add comments to counter verification plan
Signed-off-by: Paul Zavalney <paul.zavalney@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_Counters.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_Counters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\core-v-docs\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\pazavaln\reference\openhw\docs\pauls_fork\core-v-docs\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DD387A-3F96-4D0F-BB17-6865E9E20682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D1B6A4-4AF4-484F-8DE6-7626F954B4D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21920" yWindow="2060" windowWidth="16600" windowHeight="10160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CV32E40P Counters" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -347,14 +347,194 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>OVPsim ISS (Reference Model used by CV32E40P) does not support mhpcounters</t>
+    <t>[PZ] Test should also have a directed self checking component to check if instruction retired and tracer has proper signal hookup to the ISS. For example, perhaps an ebreak has a bug where it does not cause the instruction retired signal to assert and hence both the model and design do not increment the counter.
+[PZ] Test should read counter and ensure it is not reset due to a read (as CSRR is converted to CSRRSI)
+[PZ] Check writeable (perhaps coverred in CSR test)</t>
+  </si>
+  <si>
+    <t>LD_STALL</t>
+  </si>
+  <si>
+    <t>JMP_STALL</t>
+  </si>
+  <si>
+    <t>IMISS</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>BRANCH</t>
+  </si>
+  <si>
+    <t>BRANCH_TAKEN</t>
+  </si>
+  <si>
+    <t>COMP_INSTR</t>
+  </si>
+  <si>
+    <t>PIPE_STALL</t>
+  </si>
+  <si>
+    <t>APU_TYPE</t>
+  </si>
+  <si>
+    <t>APU_CONT</t>
+  </si>
+  <si>
+    <t>APU_DEP</t>
+  </si>
+  <si>
+    <t>APU_WB</t>
+  </si>
+  <si>
+    <t>platform specific event bit[2]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[3]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[4]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[5]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[6]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[7]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[8]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[9]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[10]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[11]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[12]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[13]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[14]</t>
+  </si>
+  <si>
+    <t>platform specific event bit[15]</t>
+  </si>
+  <si>
+    <t>mcountinhibit</t>
+  </si>
+  <si>
+    <t>Inhibit counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check reset value and ensure no counters are counting out of reset
+check inihibit will stop corresponding counter when set, and run when cleared
+</t>
+  </si>
+  <si>
+    <t>stopcount</t>
+  </si>
+  <si>
+    <t>RISC-V External Debug Support Version 0.13.2</t>
+  </si>
+  <si>
+    <t>Chapter 4 RISC-V Debug</t>
+  </si>
+  <si>
+    <t>stopcount is tied to 0</t>
+  </si>
+  <si>
+    <t>check counters continue to count during debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that the counter increments for each compressed instruction being retired (and not non-compressed)
+</t>
+  </si>
+  <si>
+    <t>increment for each branch instruction retired</t>
+  </si>
+  <si>
+    <t>increment for each taken jump instruction retired</t>
+  </si>
+  <si>
+    <t>cycles for pipeline being stalled due to PULP ELW instruction</t>
+  </si>
+  <si>
+    <t>Check that the counter increments for each stall cycle due to a load</t>
+  </si>
+  <si>
+    <t>Check that the counter increments for each stall cycle due to a JMP</t>
+  </si>
+  <si>
+    <t>Check that the counter increments for each clock cycle that is stalled due to fetching instruction due to memory delays (excluding cycles for JMP and BRANCHES)</t>
+  </si>
+  <si>
+    <t>increment for each Load from memory</t>
+  </si>
+  <si>
+    <t>increment for each Store to memory</t>
+  </si>
+  <si>
+    <t>increment for each branch instruction being taken is retired</t>
+  </si>
+  <si>
+    <t>[PZ] low priority</t>
+  </si>
+  <si>
+    <t>[PZ] high priority</t>
+  </si>
+  <si>
+    <t>[PZ] medium priority</t>
+  </si>
+  <si>
+    <t>[PZ] medium priority (may already be done in debug_test)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>CORE-V CV32E40P User Manual</t>
+  </si>
+  <si>
+    <t>Performance Counters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OVPsim ISS (Reference Model used by CV32E40P) does not support mhpcounters
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>[PZ] As per spec, check that if multiple events happen at the same cycle, only increment +1.
+[PZ] By default, only one event counter. Check all events can individually, separately increment counter.
+[PZ] long term, change parameter (NUM_MHPMCOUNTERS) to increase counters to maximum and randomly check if counters are implemented/counting with at least minstret</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,16 +584,28 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -442,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -492,6 +684,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,11 +714,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,11 +1164,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML10"/>
+  <dimension ref="A1:AML26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -963,7 +1179,8 @@
     <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="56.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="54.5703125" style="1" customWidth="1"/>
     <col min="11" max="1024" width="17" style="1" customWidth="1"/>
@@ -1003,10 +1220,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -1028,11 +1245,11 @@
         <v>33</v>
       </c>
       <c r="I2" s="17"/>
-      <c r="J2" s="24"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A3" s="21"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="15" t="s">
         <v>17</v>
       </c>
@@ -1052,11 +1269,11 @@
         <v>33</v>
       </c>
       <c r="I3" s="17"/>
-      <c r="J3" s="24"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A4" s="21"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="15" t="s">
         <v>18</v>
       </c>
@@ -1076,13 +1293,13 @@
         <v>33</v>
       </c>
       <c r="I4" s="17"/>
-      <c r="J4" s="24"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -1100,11 +1317,11 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="24"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="129">
-      <c r="A6" s="21"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="16" t="s">
         <v>23</v>
       </c>
@@ -1120,13 +1337,13 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="24"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" ht="128.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1148,11 +1365,11 @@
         <v>36</v>
       </c>
       <c r="I7" s="11"/>
-      <c r="J7" s="24"/>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="57">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="128.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
@@ -1172,11 +1389,13 @@
         <v>36</v>
       </c>
       <c r="I8" s="11"/>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="117">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
+      <c r="J8" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="156.75">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
@@ -1196,33 +1415,391 @@
         <v>36</v>
       </c>
       <c r="I9" s="11"/>
-      <c r="J9" s="25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="5" customFormat="1">
-      <c r="A10" s="19" t="s">
+      <c r="J9" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A10" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="42.75">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="4" customFormat="1">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="42.75">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="85.5">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="5" customFormat="1">
+      <c r="A26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A10:J10"/>
+  <mergeCells count="9">
+    <mergeCell ref="A26:J26"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A10:A24"/>
+    <mergeCell ref="B10:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1234,19 +1811,19 @@
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G9</xm:sqref>
+          <xm:sqref>G2:G25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9EE0629D-C984-46E5-B214-C9E0CDFCC0DF}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H9</xm:sqref>
+          <xm:sqref>H2:H25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{378A2363-F5F8-4E63-BBA6-5FAC23B39D93}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F9</xm:sqref>
+          <xm:sqref>F2:F25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated based on @silabs-PaulZ input
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_Counters.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_Counters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\pazavaln\reference\openhw\docs\pauls_fork\core-v-docs\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D1B6A4-4AF4-484F-8DE6-7626F954B4D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDC4624-82E1-4C3A-BE3D-185D2D9567D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21920" yWindow="2060" windowWidth="16600" windowHeight="10160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CV32E40P Counters" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -335,21 +335,7 @@
     </r>
   </si>
   <si>
-    <t>Check the value of the counter. Exercise it with different sequence of instructions.
-Test counter overflow.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check that the event 0 means no event.
-Check different combinations of events and counters. Exercise it with different sequence of instructions.
-</t>
-  </si>
-  <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>[PZ] Test should also have a directed self checking component to check if instruction retired and tracer has proper signal hookup to the ISS. For example, perhaps an ebreak has a bug where it does not cause the instruction retired signal to assert and hence both the model and design do not increment the counter.
-[PZ] Test should read counter and ensure it is not reset due to a read (as CSRR is converted to CSRRSI)
-[PZ] Check writeable (perhaps coverred in CSR test)</t>
   </si>
   <si>
     <t>LD_STALL</t>
@@ -514,27 +500,39 @@
     <t>Performance Counters</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">OVPsim ISS (Reference Model used by CV32E40P) does not support mhpcounters
+    <t>Directed self checking test to check if instruction retired and tracer has proper signal hookup to the ISS. For example, perhaps an ebreak has a bug where it does not cause the instruction retired signal to assert and hence both the model and design do not increment the counter.
+Testcase should also include the following:
+- Read counter and ensure it is not reset due to a read (as CSRR is converted to CSRRSI).
+- Exercise counter overflow.</t>
+  </si>
+  <si>
+    <t>Check the value of the counter. Exercise it with different sequence of instructions.</t>
+  </si>
+  <si>
+    <t>Test suggested by PaulZ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific checks in the Directed Test:
+- Check that the event 0 means no event.
+- Check different combinations of events and counters.
+- Check that if multiple events happen at the same cycle, only increment +1.
+- Check all events can individually, separately increment counter.
+- Use parameter NUM_MHPMCOUNTERS to increase counters to maximum and randomly check if counters are implemented/counting
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t>[PZ] As per spec, check that if multiple events happen at the same cycle, only increment +1.
-[PZ] By default, only one event counter. Check all events can individually, separately increment counter.
-[PZ] long term, change parameter (NUM_MHPMCOUNTERS) to increase counters to maximum and randomly check if counters are implemented/counting with at least minstret</t>
-    </r>
+  </si>
+  <si>
+    <t>OVPsim ISS (Reference Model used by CV32E40P) does not support mhpcounters.
+This could lead to a lot of tests…</t>
+  </si>
+  <si>
+    <t>APU not covered in CV32E40P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -596,16 +594,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <strike/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -634,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -653,9 +666,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -684,50 +694,68 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1164,11 +1192,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AML26"/>
+  <dimension ref="A1:AML27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1179,7 +1207,7 @@
     <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="56.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="54.5703125" style="1" customWidth="1"/>
@@ -1216,590 +1244,650 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A4" s="25"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="42.75">
+      <c r="A5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="129">
+      <c r="A6" s="25"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="128.25">
+      <c r="A7" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="171" customHeight="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="148.5" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A11" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A12" s="28"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A2" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="16" t="s">
+      <c r="D12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="42.75">
+      <c r="A13" s="28"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A14" s="28"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A15" s="28"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A16" s="28"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A17" s="28"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A18" s="28"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="42.75">
+      <c r="A19" s="28"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A20" s="28"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A21" s="28"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A22" s="28"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A23" s="28"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A24" s="28"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="85.5">
+      <c r="A25" s="28"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="28.5">
+      <c r="A26" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G26" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H26" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="22"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A3" s="26"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="22"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A4" s="26"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A5" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" ht="129">
-      <c r="A6" s="26"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" ht="128.25">
-      <c r="A7" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="128.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="156.75">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="28.5">
-      <c r="A10" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="28.5">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="4" customFormat="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="4" customFormat="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="4" customFormat="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="42.75">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="28.5">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="29" t="s">
+      <c r="I26" s="33"/>
+      <c r="J26" s="29" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="4" customFormat="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="85.5">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="28.5">
-      <c r="A25" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="5" customFormat="1">
-      <c r="A26" s="24" t="s">
+    <row r="27" spans="1:10" s="5" customFormat="1">
+      <c r="A27" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A27:J27"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A10:A24"/>
-    <mergeCell ref="B10:B24"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A11:A25"/>
+    <mergeCell ref="B11:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1811,19 +1899,19 @@
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G25</xm:sqref>
+          <xm:sqref>G2:G26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9EE0629D-C984-46E5-B214-C9E0CDFCC0DF}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H25</xm:sqref>
+          <xm:sqref>H2:H26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{378A2363-F5F8-4E63-BBA6-5FAC23B39D93}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F25</xm:sqref>
+          <xm:sqref>F2:F26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1847,15 +1935,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>